<commit_message>
Add function to get Excel row and col number
</commit_message>
<xml_diff>
--- a/src/test/resources/ExcelTest.xlsx
+++ b/src/test/resources/ExcelTest.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\personmalWorkspace\gitWorkSpace\ZongzheUtils\src\test\resources\foo.zongzhe.file.utils\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\personmalWorkspace\gitWorkSpace\ZongzheUtils\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE2CAEC-6B51-424E-807B-1E6AFBB4F260}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97A6B17D-B4CA-4047-BA1E-5D5B9714C383}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Column 1</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -36,6 +36,14 @@
   </si>
   <si>
     <t>String input</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>someValue</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>test for row</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -362,15 +370,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -378,7 +386,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -386,9 +394,17 @@
         <v>100</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>43344</v>
+      </c>
+      <c r="F3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>